<commit_message>
2022-05-06 Update01 1. CategoryItem Field 명칭 수정 Cate -> Item 2. CateGroup, Item 프로시저 생성 및 모델 작성 3. Frm_Info_CategoryItem CRUD 개발
</commit_message>
<xml_diff>
--- a/00. 설계/Table 설계.xlsx
+++ b/00. 설계/Table 설계.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\00.Storage\Study\Programing\Project\MES\00. 설계\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D717693-A49F-4575-8587-EDB295F9C9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB1A515-7CF2-49AC-953D-B33611AD5102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6FFB4B5A-5F32-430F-A257-1851DE962E89}"/>
+    <workbookView xWindow="28920" yWindow="2955" windowWidth="16080" windowHeight="14370" xr2:uid="{6FFB4B5A-5F32-430F-A257-1851DE962E89}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="180">
   <si>
     <t>지시수량</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -355,35 +355,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>종합코드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CateCode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Level</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>HighCate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상위 카테고리코드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>카테고리 코드</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>깊이</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CateValue</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -706,15 +686,6 @@
     <t>OrderNo</t>
   </si>
   <si>
-    <t>깊이 제한 필요or 특정 level 이하만 작성가능</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10 : 완제품,    20 : 반제품,    30 : 원자재,
-40 : 부자재,    50 : 소모자재, 60 : 개발TEST</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MC + 자재타입(16진수) + 순번 0000N</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -727,14 +698,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CI + 상위코드 + 16진수 순서(2자리)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3Level 초과 방지필요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>그룹 코드</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -748,6 +711,49 @@
   </si>
   <si>
     <t>종합코드 구분을 위한 그룹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>종합코드 - 그룹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>종합코드 - 아이템</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상위 그룹코드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HighGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CI + 16진수 순서(2자리)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR(4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ItemCode</t>
+  </si>
+  <si>
+    <t>ItemValue</t>
+  </si>
+  <si>
+    <t>01 : 완제품,    02 : 반제품,    03 : 원자재,
+04 : 부자재,    05 : 소모자재, 06 : 개발TEST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CG + 상위코드 + 16진수 순서(3자리), 최상위는 2자리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3Level 이상 방지필요</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1238,36 +1244,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1303,6 +1279,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1618,10 +1624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D18479-4FC6-49A3-AAC7-5696D0E9C401}">
-  <dimension ref="B1:H207"/>
+  <dimension ref="B1:H206"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A151" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C171" sqref="C171"/>
+      <selection activeCell="H160" sqref="H160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1631,33 +1637,33 @@
     <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.875" style="19" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="20"/>
-    <col min="8" max="8" width="42.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40" t="s">
-        <v>135</v>
-      </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
       <c r="G2" s="21"/>
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
       <c r="G3" s="7"/>
       <c r="H3" s="8"/>
     </row>
@@ -1689,13 +1695,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>17</v>
@@ -1716,16 +1722,16 @@
         <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
@@ -1739,13 +1745,13 @@
         <v>19</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>21</v>
@@ -1762,14 +1768,14 @@
         <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
@@ -1783,14 +1789,14 @@
         <v>2</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
@@ -1804,7 +1810,7 @@
         <v>12</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>16</v>
@@ -1823,14 +1829,14 @@
         <v>69</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
@@ -1844,7 +1850,7 @@
         <v>3</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>16</v>
@@ -1865,7 +1871,7 @@
         <v>4</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>16</v>
@@ -1884,7 +1890,7 @@
         <v>5</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>16</v>
@@ -1903,7 +1909,7 @@
         <v>6</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>16</v>
@@ -1924,7 +1930,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>16</v>
@@ -1943,7 +1949,7 @@
         <v>8</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>16</v>
@@ -1956,14 +1962,14 @@
       <c r="B19" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="45" t="s">
-        <v>153</v>
-      </c>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="47"/>
+      <c r="C19" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="37"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E20" s="20"/>
@@ -1972,28 +1978,28 @@
       <c r="E21" s="20"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="E22" s="29"/>
-      <c r="F22" s="30"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="E22" s="46"/>
+      <c r="F22" s="47"/>
       <c r="G22" s="21"/>
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="32"/>
-      <c r="D23" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="E23" s="34"/>
-      <c r="F23" s="35"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="43"/>
+      <c r="F23" s="44"/>
       <c r="G23" s="7"/>
       <c r="H23" s="8"/>
     </row>
@@ -2025,20 +2031,20 @@
         <v>1</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>43</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G25" s="10"/>
       <c r="H25" s="12" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
@@ -2046,10 +2052,10 @@
         <v>2</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>48</v>
@@ -2071,13 +2077,13 @@
         <v>40</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H27" s="4"/>
     </row>
@@ -2092,7 +2098,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>16</v>
@@ -2105,20 +2111,20 @@
         <v>5</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="4" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
@@ -2132,7 +2138,7 @@
         <v>12</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>16</v>
@@ -2151,14 +2157,14 @@
         <v>44</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
@@ -2172,7 +2178,7 @@
         <v>3</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>16</v>
@@ -2193,7 +2199,7 @@
         <v>4</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>16</v>
@@ -2212,7 +2218,7 @@
         <v>5</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>16</v>
@@ -2231,7 +2237,7 @@
         <v>6</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>16</v>
@@ -2252,7 +2258,7 @@
         <v>7</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>16</v>
@@ -2271,7 +2277,7 @@
         <v>8</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>16</v>
@@ -2286,39 +2292,39 @@
       <c r="B39" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="36" t="s">
-        <v>123</v>
-      </c>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="37"/>
+      <c r="C39" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="27"/>
     </row>
     <row r="41" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="42" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B42" s="26" t="s">
+      <c r="B42" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="27"/>
-      <c r="D42" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="E42" s="29"/>
-      <c r="F42" s="30"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="E42" s="46"/>
+      <c r="F42" s="47"/>
       <c r="G42" s="21"/>
       <c r="H42" s="3"/>
     </row>
     <row r="43" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="31" t="s">
+      <c r="B43" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="32"/>
-      <c r="D43" s="33" t="s">
-        <v>138</v>
-      </c>
-      <c r="E43" s="34"/>
-      <c r="F43" s="35"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="E43" s="43"/>
+      <c r="F43" s="44"/>
       <c r="G43" s="7"/>
       <c r="H43" s="8"/>
     </row>
@@ -2353,10 +2359,10 @@
         <v>22</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>17</v>
@@ -2371,20 +2377,20 @@
         <v>2</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D46" s="11" t="s">
         <v>43</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G46" s="10"/>
       <c r="H46" s="12" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.3">
@@ -2392,10 +2398,10 @@
         <v>3</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>48</v>
@@ -2417,13 +2423,13 @@
         <v>40</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H48" s="4"/>
     </row>
@@ -2438,7 +2444,7 @@
         <v>0</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>16</v>
@@ -2454,10 +2460,10 @@
         <v>28</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>16</v>
@@ -2478,7 +2484,7 @@
         <v>12</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>16</v>
@@ -2497,14 +2503,14 @@
         <v>44</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.3">
@@ -2518,7 +2524,7 @@
         <v>3</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>16</v>
@@ -2539,7 +2545,7 @@
         <v>4</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>16</v>
@@ -2558,7 +2564,7 @@
         <v>5</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>16</v>
@@ -2577,7 +2583,7 @@
         <v>6</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>16</v>
@@ -2598,7 +2604,7 @@
         <v>7</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>16</v>
@@ -2617,7 +2623,7 @@
         <v>8</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>16</v>
@@ -2633,14 +2639,14 @@
       <c r="B60" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C60" s="36" t="s">
-        <v>141</v>
-      </c>
-      <c r="D60" s="36"/>
-      <c r="E60" s="36"/>
-      <c r="F60" s="36"/>
-      <c r="G60" s="36"/>
-      <c r="H60" s="37"/>
+      <c r="C60" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="D60" s="26"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="26"/>
+      <c r="G60" s="26"/>
+      <c r="H60" s="27"/>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E61" s="23"/>
@@ -2651,28 +2657,28 @@
       <c r="G62" s="23"/>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B63" s="38" t="s">
+      <c r="B63" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C63" s="39"/>
-      <c r="D63" s="40" t="s">
-        <v>143</v>
-      </c>
-      <c r="E63" s="40"/>
-      <c r="F63" s="40"/>
+      <c r="C63" s="29"/>
+      <c r="D63" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="E63" s="30"/>
+      <c r="F63" s="30"/>
       <c r="G63" s="21"/>
       <c r="H63" s="3"/>
     </row>
     <row r="64" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="41" t="s">
+      <c r="B64" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C64" s="42"/>
-      <c r="D64" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="E64" s="43"/>
-      <c r="F64" s="43"/>
+      <c r="C64" s="32"/>
+      <c r="D64" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="E64" s="33"/>
+      <c r="F64" s="33"/>
       <c r="G64" s="7"/>
       <c r="H64" s="8"/>
     </row>
@@ -2710,7 +2716,7 @@
         <v>14</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F66" s="10" t="s">
         <v>17</v>
@@ -2725,20 +2731,20 @@
         <v>2</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D67" s="11" t="s">
         <v>43</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G67" s="2"/>
       <c r="H67" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.3">
@@ -2746,10 +2752,10 @@
         <v>3</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>48</v>
@@ -2759,7 +2765,7 @@
       </c>
       <c r="G68" s="2"/>
       <c r="H68" s="4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.3">
@@ -2773,13 +2779,13 @@
         <v>40</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H69" s="4"/>
     </row>
@@ -2794,14 +2800,14 @@
         <v>0</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G70" s="2"/>
       <c r="H70" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.3">
@@ -2812,10 +2818,10 @@
         <v>56</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>16</v>
@@ -2830,20 +2836,20 @@
         <v>7</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E72" s="24" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F72" s="24" t="s">
         <v>16</v>
       </c>
       <c r="G72" s="24"/>
       <c r="H72" s="25" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.3">
@@ -2857,7 +2863,7 @@
         <v>12</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>16</v>
@@ -2873,17 +2879,17 @@
         <v>30</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G74" s="2"/>
       <c r="H74" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.3">
@@ -2897,7 +2903,7 @@
         <v>3</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>16</v>
@@ -2918,7 +2924,7 @@
         <v>4</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>16</v>
@@ -2937,7 +2943,7 @@
         <v>5</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>16</v>
@@ -2956,7 +2962,7 @@
         <v>6</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>16</v>
@@ -2977,7 +2983,7 @@
         <v>7</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>16</v>
@@ -2996,7 +3002,7 @@
         <v>8</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F80" s="7" t="s">
         <v>16</v>
@@ -3012,14 +3018,14 @@
       <c r="B82" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C82" s="44" t="s">
-        <v>125</v>
-      </c>
-      <c r="D82" s="36"/>
-      <c r="E82" s="36"/>
-      <c r="F82" s="36"/>
-      <c r="G82" s="36"/>
-      <c r="H82" s="37"/>
+      <c r="C82" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="D82" s="26"/>
+      <c r="E82" s="26"/>
+      <c r="F82" s="26"/>
+      <c r="G82" s="26"/>
+      <c r="H82" s="27"/>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E83" s="20"/>
@@ -3028,28 +3034,28 @@
       <c r="E84" s="20"/>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B85" s="38" t="s">
+      <c r="B85" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C85" s="39"/>
-      <c r="D85" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="E85" s="40"/>
-      <c r="F85" s="40"/>
+      <c r="C85" s="29"/>
+      <c r="D85" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="E85" s="30"/>
+      <c r="F85" s="30"/>
       <c r="G85" s="21"/>
       <c r="H85" s="3"/>
     </row>
     <row r="86" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B86" s="41" t="s">
+      <c r="B86" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C86" s="42"/>
-      <c r="D86" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="E86" s="43"/>
-      <c r="F86" s="43"/>
+      <c r="C86" s="32"/>
+      <c r="D86" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="E86" s="33"/>
+      <c r="F86" s="33"/>
       <c r="G86" s="7"/>
       <c r="H86" s="8"/>
     </row>
@@ -3081,22 +3087,22 @@
         <v>1</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D88" s="11" t="s">
         <v>43</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H88" s="12" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.3">
@@ -3129,16 +3135,16 @@
         <v>41</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H90" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.3">
@@ -3152,13 +3158,13 @@
         <v>40</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H91" s="4"/>
     </row>
@@ -3173,7 +3179,7 @@
         <v>0</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F92" s="2" t="s">
         <v>16</v>
@@ -3186,20 +3192,20 @@
         <v>6</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E93" s="24" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G93" s="2"/>
       <c r="H93" s="25" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.3">
@@ -3213,7 +3219,7 @@
         <v>12</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>16</v>
@@ -3232,14 +3238,14 @@
         <v>44</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G95" s="2"/>
       <c r="H95" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.3">
@@ -3253,7 +3259,7 @@
         <v>3</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>16</v>
@@ -3274,7 +3280,7 @@
         <v>4</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>16</v>
@@ -3293,7 +3299,7 @@
         <v>5</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F98" s="2" t="s">
         <v>16</v>
@@ -3312,7 +3318,7 @@
         <v>6</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F99" s="2" t="s">
         <v>16</v>
@@ -3333,7 +3339,7 @@
         <v>7</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F100" s="2" t="s">
         <v>16</v>
@@ -3352,7 +3358,7 @@
         <v>8</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F101" s="7" t="s">
         <v>16</v>
@@ -3368,14 +3374,14 @@
       <c r="B103" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C103" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="D103" s="36"/>
-      <c r="E103" s="36"/>
-      <c r="F103" s="36"/>
-      <c r="G103" s="36"/>
-      <c r="H103" s="37"/>
+      <c r="C103" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="D103" s="26"/>
+      <c r="E103" s="26"/>
+      <c r="F103" s="26"/>
+      <c r="G103" s="26"/>
+      <c r="H103" s="27"/>
     </row>
     <row r="104" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E104" s="22"/>
@@ -3383,28 +3389,28 @@
     </row>
     <row r="105" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="106" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B106" s="38" t="s">
+      <c r="B106" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C106" s="39"/>
-      <c r="D106" s="40" t="s">
-        <v>149</v>
-      </c>
-      <c r="E106" s="40"/>
-      <c r="F106" s="40"/>
+      <c r="C106" s="29"/>
+      <c r="D106" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="E106" s="30"/>
+      <c r="F106" s="30"/>
       <c r="G106" s="21"/>
       <c r="H106" s="3"/>
     </row>
     <row r="107" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B107" s="41" t="s">
+      <c r="B107" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C107" s="42"/>
-      <c r="D107" s="43" t="s">
-        <v>159</v>
-      </c>
-      <c r="E107" s="43"/>
-      <c r="F107" s="43"/>
+      <c r="C107" s="32"/>
+      <c r="D107" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="E107" s="33"/>
+      <c r="F107" s="33"/>
       <c r="G107" s="7"/>
       <c r="H107" s="8"/>
     </row>
@@ -3436,13 +3442,13 @@
         <v>1</v>
       </c>
       <c r="C109" s="11" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F109" s="10" t="s">
         <v>17</v>
@@ -3451,7 +3457,7 @@
         <v>18</v>
       </c>
       <c r="H109" s="12" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="110" spans="2:8" x14ac:dyDescent="0.3">
@@ -3459,13 +3465,13 @@
         <v>2</v>
       </c>
       <c r="C110" s="11" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D110" s="11" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F110" s="2" t="s">
         <v>16</v>
@@ -3476,13 +3482,13 @@
     <row r="111" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B111" s="9"/>
       <c r="C111" s="11" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D111" s="11" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F111" s="2" t="s">
         <v>16</v>
@@ -3495,10 +3501,10 @@
         <v>3</v>
       </c>
       <c r="C112" s="11" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>48</v>
@@ -3508,7 +3514,7 @@
       </c>
       <c r="G112" s="10"/>
       <c r="H112" s="17" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
     </row>
     <row r="113" spans="2:8" x14ac:dyDescent="0.3">
@@ -3516,13 +3522,13 @@
         <v>4</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F113" s="2" t="s">
         <v>16</v>
@@ -3538,10 +3544,10 @@
         <v>50</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F114" s="2" t="s">
         <v>16</v>
@@ -3560,14 +3566,14 @@
         <v>51</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F115" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G115" s="2"/>
       <c r="H115" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="116" spans="2:8" x14ac:dyDescent="0.3">
@@ -3581,7 +3587,7 @@
         <v>69</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F116" s="2" t="s">
         <v>16</v>
@@ -3600,7 +3606,7 @@
         <v>12</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F117" s="2" t="s">
         <v>16</v>
@@ -3619,7 +3625,7 @@
         <v>3</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F118" s="2" t="s">
         <v>16</v>
@@ -3640,7 +3646,7 @@
         <v>4</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F119" s="2" t="s">
         <v>16</v>
@@ -3659,7 +3665,7 @@
         <v>5</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F120" s="2" t="s">
         <v>16</v>
@@ -3678,7 +3684,7 @@
         <v>6</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F121" s="2" t="s">
         <v>16</v>
@@ -3699,7 +3705,7 @@
         <v>7</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F122" s="2" t="s">
         <v>16</v>
@@ -3718,7 +3724,7 @@
         <v>8</v>
       </c>
       <c r="E123" s="7" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F123" s="7" t="s">
         <v>16</v>
@@ -3731,39 +3737,39 @@
       <c r="B125" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C125" s="44" t="s">
-        <v>97</v>
-      </c>
-      <c r="D125" s="36"/>
-      <c r="E125" s="36"/>
-      <c r="F125" s="36"/>
-      <c r="G125" s="36"/>
-      <c r="H125" s="37"/>
+      <c r="C125" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="D125" s="26"/>
+      <c r="E125" s="26"/>
+      <c r="F125" s="26"/>
+      <c r="G125" s="26"/>
+      <c r="H125" s="27"/>
     </row>
     <row r="127" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="128" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B128" s="38" t="s">
+      <c r="B128" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C128" s="39"/>
-      <c r="D128" s="40" t="s">
-        <v>150</v>
-      </c>
-      <c r="E128" s="40"/>
-      <c r="F128" s="40"/>
+      <c r="C128" s="29"/>
+      <c r="D128" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="E128" s="30"/>
+      <c r="F128" s="30"/>
       <c r="G128" s="21"/>
       <c r="H128" s="3"/>
     </row>
     <row r="129" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B129" s="41" t="s">
+      <c r="B129" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C129" s="42"/>
-      <c r="D129" s="43" t="s">
+      <c r="C129" s="32"/>
+      <c r="D129" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="E129" s="43"/>
-      <c r="F129" s="43"/>
+      <c r="E129" s="33"/>
+      <c r="F129" s="33"/>
       <c r="G129" s="7"/>
       <c r="H129" s="8"/>
     </row>
@@ -3801,7 +3807,7 @@
         <v>51</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F131" s="10" t="s">
         <v>17</v>
@@ -3822,7 +3828,7 @@
         <v>57</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F132" s="2" t="s">
         <v>16</v>
@@ -3848,7 +3854,7 @@
       </c>
       <c r="G133" s="10"/>
       <c r="H133" s="17" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="134" spans="2:8" x14ac:dyDescent="0.3">
@@ -3862,7 +3868,7 @@
         <v>60</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F134" s="2" t="s">
         <v>16</v>
@@ -3881,7 +3887,7 @@
         <v>61</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F135" s="2" t="s">
         <v>16</v>
@@ -3900,7 +3906,7 @@
         <v>62</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F136" s="2" t="s">
         <v>16</v>
@@ -3919,7 +3925,7 @@
         <v>63</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F137" s="2" t="s">
         <v>16</v>
@@ -3938,7 +3944,7 @@
         <v>64</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F138" s="2" t="s">
         <v>16</v>
@@ -3957,7 +3963,7 @@
         <v>65</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F139" s="2" t="s">
         <v>16</v>
@@ -3976,7 +3982,7 @@
         <v>66</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F140" s="2" t="s">
         <v>16</v>
@@ -3995,7 +4001,7 @@
         <v>67</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F141" s="2" t="s">
         <v>16</v>
@@ -4014,7 +4020,7 @@
         <v>68</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F142" s="2" t="s">
         <v>16</v>
@@ -4033,7 +4039,7 @@
         <v>69</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F143" s="2" t="s">
         <v>16</v>
@@ -4052,7 +4058,7 @@
         <v>12</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F144" s="2" t="s">
         <v>16</v>
@@ -4071,7 +4077,7 @@
         <v>3</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F145" s="2" t="s">
         <v>16</v>
@@ -4092,7 +4098,7 @@
         <v>4</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F146" s="2" t="s">
         <v>16</v>
@@ -4111,7 +4117,7 @@
         <v>5</v>
       </c>
       <c r="E147" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F147" s="2" t="s">
         <v>16</v>
@@ -4130,7 +4136,7 @@
         <v>6</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F148" s="2" t="s">
         <v>16</v>
@@ -4151,7 +4157,7 @@
         <v>7</v>
       </c>
       <c r="E149" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F149" s="2" t="s">
         <v>16</v>
@@ -4170,7 +4176,7 @@
         <v>8</v>
       </c>
       <c r="E150" s="7" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F150" s="7" t="s">
         <v>16</v>
@@ -4183,37 +4189,37 @@
       <c r="B152" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C152" s="36"/>
-      <c r="D152" s="36"/>
-      <c r="E152" s="36"/>
-      <c r="F152" s="36"/>
-      <c r="G152" s="36"/>
-      <c r="H152" s="37"/>
+      <c r="C152" s="26"/>
+      <c r="D152" s="26"/>
+      <c r="E152" s="26"/>
+      <c r="F152" s="26"/>
+      <c r="G152" s="26"/>
+      <c r="H152" s="27"/>
     </row>
     <row r="154" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="155" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B155" s="38" t="s">
+      <c r="B155" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C155" s="39"/>
-      <c r="D155" s="40" t="s">
-        <v>170</v>
-      </c>
-      <c r="E155" s="40"/>
-      <c r="F155" s="40"/>
+      <c r="C155" s="29"/>
+      <c r="D155" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="E155" s="30"/>
+      <c r="F155" s="30"/>
       <c r="G155" s="21"/>
       <c r="H155" s="3"/>
     </row>
     <row r="156" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B156" s="41" t="s">
+      <c r="B156" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C156" s="42"/>
-      <c r="D156" s="43" t="s">
-        <v>80</v>
-      </c>
-      <c r="E156" s="43"/>
-      <c r="F156" s="43"/>
+      <c r="C156" s="32"/>
+      <c r="D156" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="E156" s="33"/>
+      <c r="F156" s="33"/>
       <c r="G156" s="7"/>
       <c r="H156" s="8"/>
     </row>
@@ -4245,13 +4251,13 @@
         <v>1</v>
       </c>
       <c r="C158" s="11" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E158" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F158" s="10" t="s">
         <v>17</v>
@@ -4260,7 +4266,7 @@
         <v>18</v>
       </c>
       <c r="H158" s="12" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="159" spans="2:8" x14ac:dyDescent="0.3">
@@ -4268,20 +4274,20 @@
         <v>2</v>
       </c>
       <c r="C159" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D159" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="D159" s="11" t="s">
-        <v>86</v>
-      </c>
       <c r="E159" s="10" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F159" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G159" s="10"/>
       <c r="H159" s="12" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
     <row r="160" spans="2:8" x14ac:dyDescent="0.3">
@@ -4289,13 +4295,13 @@
         <v>3</v>
       </c>
       <c r="C160" s="11" t="s">
-        <v>83</v>
+        <v>172</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>84</v>
+        <v>171</v>
       </c>
       <c r="E160" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F160" s="2" t="s">
         <v>16</v>
@@ -4308,13 +4314,13 @@
         <v>4</v>
       </c>
       <c r="C161" s="18" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="D161" s="18" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="E161" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F161" s="2" t="s">
         <v>16</v>
@@ -4333,7 +4339,7 @@
         <v>69</v>
       </c>
       <c r="E162" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F162" s="2" t="s">
         <v>16</v>
@@ -4352,7 +4358,7 @@
         <v>3</v>
       </c>
       <c r="E163" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F163" s="2" t="s">
         <v>16</v>
@@ -4373,7 +4379,7 @@
         <v>4</v>
       </c>
       <c r="E164" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F164" s="2" t="s">
         <v>16</v>
@@ -4392,7 +4398,7 @@
         <v>5</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F165" s="2" t="s">
         <v>16</v>
@@ -4411,7 +4417,7 @@
         <v>6</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F166" s="2" t="s">
         <v>16</v>
@@ -4432,7 +4438,7 @@
         <v>7</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F167" s="2" t="s">
         <v>16</v>
@@ -4451,7 +4457,7 @@
         <v>8</v>
       </c>
       <c r="E168" s="7" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F168" s="7" t="s">
         <v>16</v>
@@ -4464,42 +4470,42 @@
       <c r="B170" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C170" s="36" t="s">
-        <v>177</v>
-      </c>
-      <c r="D170" s="36"/>
-      <c r="E170" s="36"/>
-      <c r="F170" s="36"/>
-      <c r="G170" s="36"/>
-      <c r="H170" s="37"/>
+      <c r="C170" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="D170" s="26"/>
+      <c r="E170" s="26"/>
+      <c r="F170" s="26"/>
+      <c r="G170" s="26"/>
+      <c r="H170" s="27"/>
     </row>
     <row r="172" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E172" s="23"/>
       <c r="G172" s="23"/>
     </row>
     <row r="173" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B173" s="38" t="s">
+      <c r="B173" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C173" s="39"/>
-      <c r="D173" s="40" t="s">
-        <v>151</v>
-      </c>
-      <c r="E173" s="40"/>
-      <c r="F173" s="40"/>
+      <c r="C173" s="29"/>
+      <c r="D173" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="E173" s="30"/>
+      <c r="F173" s="30"/>
       <c r="G173" s="21"/>
       <c r="H173" s="3"/>
     </row>
     <row r="174" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B174" s="41" t="s">
+      <c r="B174" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C174" s="42"/>
-      <c r="D174" s="43" t="s">
-        <v>80</v>
-      </c>
-      <c r="E174" s="43"/>
-      <c r="F174" s="43"/>
+      <c r="C174" s="32"/>
+      <c r="D174" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="E174" s="33"/>
+      <c r="F174" s="33"/>
       <c r="G174" s="7"/>
       <c r="H174" s="8"/>
     </row>
@@ -4531,20 +4537,18 @@
         <v>1</v>
       </c>
       <c r="C176" s="11" t="s">
-        <v>81</v>
+        <v>164</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>85</v>
+        <v>171</v>
       </c>
       <c r="E176" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F176" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G176" s="10" t="s">
-        <v>18</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="F176" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G176" s="10"/>
       <c r="H176" s="12"/>
     </row>
     <row r="177" spans="2:8" x14ac:dyDescent="0.3">
@@ -4552,34 +4556,34 @@
         <v>2</v>
       </c>
       <c r="C177" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D177" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E177" s="10" t="s">
-        <v>102</v>
+        <v>175</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E177" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="F177" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G177" s="10"/>
       <c r="H177" s="12" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
     </row>
     <row r="178" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B178" s="9">
         <v>3</v>
       </c>
-      <c r="C178" s="11" t="s">
+      <c r="C178" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="D178" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D178" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="E178" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F178" s="2" t="s">
         <v>16</v>
@@ -4591,33 +4595,33 @@
       <c r="B179" s="9">
         <v>4</v>
       </c>
-      <c r="C179" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="D179" s="18" t="s">
-        <v>88</v>
+      <c r="C179" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="E179" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F179" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G179" s="10"/>
-      <c r="H179" s="17"/>
+      <c r="G179" s="2"/>
+      <c r="H179" s="4"/>
     </row>
     <row r="180" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B180" s="9">
         <v>5</v>
       </c>
-      <c r="C180" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D180" s="1" t="s">
-        <v>12</v>
+      <c r="C180" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D180" s="18" t="s">
+        <v>69</v>
       </c>
       <c r="E180" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F180" s="2" t="s">
         <v>16</v>
@@ -4629,54 +4633,54 @@
       <c r="B181" s="9">
         <v>6</v>
       </c>
-      <c r="C181" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="D181" s="18" t="s">
-        <v>69</v>
+      <c r="C181" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="E181" s="2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="F181" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G181" s="2"/>
-      <c r="H181" s="4"/>
+      <c r="H181" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="182" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B182" s="9">
         <v>7</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E182" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F182" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G182" s="2"/>
-      <c r="H182" s="4" t="s">
-        <v>42</v>
-      </c>
+      <c r="H182" s="4"/>
     </row>
     <row r="183" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B183" s="9">
         <v>8</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E183" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F183" s="2" t="s">
         <v>16</v>
@@ -4689,226 +4693,226 @@
         <v>9</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E184" s="2" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="F184" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G184" s="2"/>
-      <c r="H184" s="4"/>
+      <c r="H184" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="185" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B185" s="9">
         <v>10</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E185" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F185" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G185" s="2"/>
-      <c r="H185" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="186" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H185" s="4"/>
+    </row>
+    <row r="186" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B186" s="9">
         <v>11</v>
       </c>
-      <c r="C186" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D186" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E186" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F186" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G186" s="2"/>
-      <c r="H186" s="4"/>
+      <c r="C186" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D186" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E186" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F186" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G186" s="7"/>
+      <c r="H186" s="8"/>
     </row>
     <row r="187" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B187" s="9">
+      <c r="E187" s="23"/>
+      <c r="G187" s="23"/>
+    </row>
+    <row r="188" spans="2:8" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B188" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C187" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D187" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E187" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F187" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G187" s="7"/>
-      <c r="H187" s="8"/>
-    </row>
-    <row r="188" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E188" s="23"/>
-      <c r="G188" s="23"/>
-    </row>
-    <row r="189" spans="2:8" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B189" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C189" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="D189" s="36"/>
-      <c r="E189" s="36"/>
-      <c r="F189" s="36"/>
-      <c r="G189" s="36"/>
-      <c r="H189" s="37"/>
-    </row>
-    <row r="190" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C188" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D188" s="26"/>
+      <c r="E188" s="26"/>
+      <c r="F188" s="26"/>
+      <c r="G188" s="26"/>
+      <c r="H188" s="27"/>
+    </row>
+    <row r="189" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="E189" s="23"/>
+      <c r="G189" s="23"/>
+    </row>
+    <row r="190" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E190" s="23"/>
       <c r="G190" s="23"/>
     </row>
-    <row r="191" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E191" s="23"/>
-      <c r="G191" s="23"/>
-    </row>
-    <row r="192" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B192" s="26" t="s">
+    <row r="191" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B191" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C192" s="27"/>
-      <c r="D192" s="28" t="s">
-        <v>152</v>
-      </c>
-      <c r="E192" s="29"/>
-      <c r="F192" s="30"/>
-      <c r="G192" s="21"/>
-      <c r="H192" s="3"/>
+      <c r="C191" s="41"/>
+      <c r="D191" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="E191" s="46"/>
+      <c r="F191" s="47"/>
+      <c r="G191" s="21"/>
+      <c r="H191" s="3"/>
+    </row>
+    <row r="192" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B192" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="C192" s="39"/>
+      <c r="D192" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="E192" s="43"/>
+      <c r="F192" s="44"/>
+      <c r="G192" s="7"/>
+      <c r="H192" s="8"/>
     </row>
     <row r="193" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B193" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C193" s="32"/>
-      <c r="D193" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="E193" s="34"/>
-      <c r="F193" s="35"/>
-      <c r="G193" s="7"/>
-      <c r="H193" s="8"/>
-    </row>
-    <row r="194" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B194" s="14" t="s">
+      <c r="B193" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C194" s="15" t="s">
+      <c r="C193" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D194" s="15" t="s">
+      <c r="D193" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E194" s="15" t="s">
+      <c r="E193" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F194" s="15" t="s">
+      <c r="F193" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G194" s="15" t="s">
+      <c r="G193" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H194" s="16" t="s">
+      <c r="H193" s="16" t="s">
         <v>12</v>
       </c>
+    </row>
+    <row r="194" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B194" s="9">
+        <v>1</v>
+      </c>
+      <c r="C194" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E194" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F194" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G194" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H194" s="12"/>
     </row>
     <row r="195" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B195" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C195" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="D195" s="1" t="s">
-        <v>41</v>
+        <v>123</v>
+      </c>
+      <c r="D195" s="11" t="s">
+        <v>88</v>
       </c>
       <c r="E195" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F195" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G195" s="10" t="s">
-        <v>18</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="F195" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G195" s="10"/>
       <c r="H195" s="12"/>
     </row>
     <row r="196" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B196" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C196" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="D196" s="11" t="s">
-        <v>93</v>
+        <v>124</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="E196" s="2" t="s">
-        <v>105</v>
+        <v>48</v>
       </c>
       <c r="F196" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G196" s="10"/>
-      <c r="H196" s="12"/>
+      <c r="H196" s="17" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="197" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B197" s="9">
-        <v>3</v>
-      </c>
-      <c r="C197" s="11" t="s">
-        <v>129</v>
+        <v>4</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>91</v>
+        <v>12</v>
       </c>
       <c r="E197" s="2" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="F197" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G197" s="10"/>
-      <c r="H197" s="17" t="s">
-        <v>92</v>
-      </c>
+      <c r="G197" s="2"/>
+      <c r="H197" s="4"/>
     </row>
     <row r="198" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B198" s="9">
-        <v>4</v>
-      </c>
-      <c r="C198" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D198" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
+      </c>
+      <c r="C198" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D198" s="18" t="s">
+        <v>69</v>
       </c>
       <c r="E198" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F198" s="2" t="s">
         <v>16</v>
@@ -4918,56 +4922,56 @@
     </row>
     <row r="199" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B199" s="9">
-        <v>5</v>
-      </c>
-      <c r="C199" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="D199" s="18" t="s">
-        <v>69</v>
+        <v>6</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="E199" s="2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="F199" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G199" s="2"/>
-      <c r="H199" s="4"/>
+      <c r="H199" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="200" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B200" s="9">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E200" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F200" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G200" s="2"/>
-      <c r="H200" s="4" t="s">
-        <v>42</v>
-      </c>
+      <c r="H200" s="4"/>
     </row>
     <row r="201" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B201" s="9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E201" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F201" s="2" t="s">
         <v>16</v>
@@ -4977,108 +4981,109 @@
     </row>
     <row r="202" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B202" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E202" s="2" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="F202" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G202" s="2"/>
-      <c r="H202" s="4"/>
+      <c r="H202" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="203" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B203" s="9">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E203" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F203" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G203" s="2"/>
-      <c r="H203" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="204" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H203" s="4"/>
+    </row>
+    <row r="204" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B204" s="9">
-        <v>10</v>
-      </c>
-      <c r="C204" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D204" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E204" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F204" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G204" s="2"/>
-      <c r="H204" s="4"/>
-    </row>
-    <row r="205" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B205" s="9">
         <v>11</v>
       </c>
-      <c r="C205" s="6" t="s">
+      <c r="C204" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D205" s="6" t="s">
+      <c r="D204" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E205" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F205" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G205" s="7"/>
-      <c r="H205" s="8"/>
-    </row>
-    <row r="206" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="207" spans="2:8" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B207" s="13" t="s">
+      <c r="E204" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F204" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G204" s="7"/>
+      <c r="H204" s="8"/>
+    </row>
+    <row r="205" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="206" spans="2:8" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B206" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C207" s="44" t="s">
-        <v>94</v>
-      </c>
-      <c r="D207" s="36"/>
-      <c r="E207" s="36"/>
-      <c r="F207" s="36"/>
-      <c r="G207" s="36"/>
-      <c r="H207" s="37"/>
+      <c r="C206" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="D206" s="26"/>
+      <c r="E206" s="26"/>
+      <c r="F206" s="26"/>
+      <c r="G206" s="26"/>
+      <c r="H206" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="C189:H189"/>
-    <mergeCell ref="B173:C173"/>
-    <mergeCell ref="D173:F173"/>
-    <mergeCell ref="B174:C174"/>
-    <mergeCell ref="D174:F174"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="D63:F63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="D64:F64"/>
-    <mergeCell ref="C82:H82"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="C60:H60"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="D85:F85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="D86:F86"/>
+    <mergeCell ref="C103:H103"/>
+    <mergeCell ref="B191:C191"/>
+    <mergeCell ref="D191:F191"/>
+    <mergeCell ref="B192:C192"/>
+    <mergeCell ref="D192:F192"/>
+    <mergeCell ref="C206:H206"/>
+    <mergeCell ref="B155:C155"/>
+    <mergeCell ref="D155:F155"/>
+    <mergeCell ref="B156:C156"/>
+    <mergeCell ref="D156:F156"/>
+    <mergeCell ref="C170:H170"/>
+    <mergeCell ref="B128:C128"/>
+    <mergeCell ref="D128:F128"/>
+    <mergeCell ref="B129:C129"/>
+    <mergeCell ref="D129:F129"/>
+    <mergeCell ref="C152:H152"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="D106:F106"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="D107:F107"/>
+    <mergeCell ref="C125:H125"/>
     <mergeCell ref="C39:H39"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -5089,36 +5094,16 @@
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="D22:F22"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="D106:F106"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="D107:F107"/>
-    <mergeCell ref="C125:H125"/>
-    <mergeCell ref="B128:C128"/>
-    <mergeCell ref="D128:F128"/>
-    <mergeCell ref="B129:C129"/>
-    <mergeCell ref="D129:F129"/>
-    <mergeCell ref="C152:H152"/>
-    <mergeCell ref="B155:C155"/>
-    <mergeCell ref="D155:F155"/>
-    <mergeCell ref="B156:C156"/>
-    <mergeCell ref="D156:F156"/>
-    <mergeCell ref="C170:H170"/>
-    <mergeCell ref="B192:C192"/>
-    <mergeCell ref="D192:F192"/>
-    <mergeCell ref="B193:C193"/>
-    <mergeCell ref="D193:F193"/>
-    <mergeCell ref="C207:H207"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="D85:F85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="D86:F86"/>
-    <mergeCell ref="C103:H103"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="C60:H60"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="D63:F63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="D64:F64"/>
+    <mergeCell ref="C82:H82"/>
+    <mergeCell ref="C188:H188"/>
+    <mergeCell ref="B173:C173"/>
+    <mergeCell ref="D173:F173"/>
+    <mergeCell ref="B174:C174"/>
+    <mergeCell ref="D174:F174"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>